<commit_message>
Finished TST1352, TST1119, TST568, TST809 and TST589.
</commit_message>
<xml_diff>
--- a/NformTester/NformTester/Keywordscripts/TST494_UserCanNotConfigureWriteDataActionWithoutPermission.xlsx
+++ b/NformTester/NformTester/Keywordscripts/TST494_UserCanNotConfigureWriteDataActionWithoutPermission.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-2415" yWindow="15" windowWidth="15480" windowHeight="11655"/>
@@ -1209,7 +1209,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7494" uniqueCount="857">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7494" uniqueCount="858">
   <si>
     <t>FormLogin_to_LiebertR_Nform</t>
   </si>
@@ -3861,6 +3861,10 @@
   <si>
     <t>T</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>;T</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -4825,8 +4829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -6200,7 +6204,7 @@
         <v>49</v>
       </c>
       <c r="D50" s="18" t="s">
-        <v>839</v>
+        <v>857</v>
       </c>
       <c r="E50" s="5" t="s">
         <v>18</v>

</xml_diff>